<commit_message>
Editex excel function (7 sec to run)
</commit_message>
<xml_diff>
--- a/AllTags.xlsx
+++ b/AllTags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.MAC.Final-1.2-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45927D7D-40E5-4389-8341-D9B0A4C54281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D197CE89-DE83-4BE5-8C3A-3397D5B58B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="19185" windowHeight="10065" xr2:uid="{9A36AAE4-B7EF-40CF-A5D5-4FCE702BA98B}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="19185" windowHeight="10065" xr2:uid="{23CD74E2-8BAE-4948-B7DD-E928CA35BAC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -1137,7 +1137,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01CF551-5B69-47F4-A158-CFC379D548F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157B1FF9-150D-4CE8-BA21-B93E6EF0AC98}">
   <dimension ref="A1:R418"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>